<commit_message>
Simulation results used for capstone poster
</commit_message>
<xml_diff>
--- a/Fuel-Station-Summary.xlsx
+++ b/Fuel-Station-Summary.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uofwaterloo-my.sharepoint.com/personal/a39nair_uwaterloo_ca/Documents/Documents/NAIR/Projects/H2-Refuelling-Capstone/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="11_08B5219C9F45860F623554765808AE7F91B982A7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D20A0D85-E097-4776-A4A7-F6DEA952C7C8}"/>
+  <xr:revisionPtr revIDLastSave="26" documentId="11_08B5F704DE67DE0E623554765860F6FB9E3983D2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{039DE419-3BCB-4347-8E9F-B7C993C5E3B0}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$J$25</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Station</t>
   </si>
@@ -59,9 +62,6 @@
     <t>Total Trucks Refuelled</t>
   </si>
   <si>
-    <t>Station Reliability</t>
-  </si>
-  <si>
     <t>Station 1</t>
   </si>
   <si>
@@ -92,7 +92,40 @@
     <t>Station 11</t>
   </si>
   <si>
-    <t>Station 12</t>
+    <t>Station Name</t>
+  </si>
+  <si>
+    <t>Tilbury North</t>
+  </si>
+  <si>
+    <t>Cambridge E</t>
+  </si>
+  <si>
+    <t>Mallorytown E</t>
+  </si>
+  <si>
+    <t>Newcastle</t>
+  </si>
+  <si>
+    <t>Cambridge W</t>
+  </si>
+  <si>
+    <t>Woodstock</t>
+  </si>
+  <si>
+    <t>Ingersoll</t>
+  </si>
+  <si>
+    <t>Port Hope</t>
+  </si>
+  <si>
+    <t>Mallorytown W</t>
+  </si>
+  <si>
+    <t>Tillbury South</t>
+  </si>
+  <si>
+    <t>Reliability</t>
   </si>
 </sst>
 </file>
@@ -111,7 +144,6 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -456,24 +488,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="132" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="21.140625" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.85546875" customWidth="1"/>
+    <col min="10" max="10" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -499,329 +529,338 @@
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
       <c r="B2">
-        <v>129</v>
+        <v>145</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
       <c r="D2">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="E2">
         <v>2</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G2">
-        <v>174</v>
+        <v>188</v>
       </c>
       <c r="H2">
-        <v>119</v>
-      </c>
-      <c r="I2">
-        <v>68.391000000000005</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+      <c r="I2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J2">
+        <v>89.893999999999991</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3">
+        <v>1814</v>
+      </c>
+      <c r="C3">
+        <v>927</v>
+      </c>
+      <c r="D3">
+        <v>1314</v>
+      </c>
+      <c r="E3">
+        <v>41</v>
+      </c>
+      <c r="F3">
+        <v>40</v>
+      </c>
+      <c r="G3">
+        <v>4099</v>
+      </c>
+      <c r="H3">
+        <v>4007</v>
+      </c>
+      <c r="I3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3">
+        <v>97.756</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4">
+        <v>274</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>94</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4">
+        <v>272</v>
+      </c>
+      <c r="H4">
+        <v>233</v>
+      </c>
+      <c r="I4" t="s">
+        <v>27</v>
+      </c>
+      <c r="J4">
+        <v>85.662000000000006</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>1972</v>
+      </c>
+      <c r="C5">
+        <v>1019</v>
+      </c>
+      <c r="D5">
+        <v>1548</v>
+      </c>
+      <c r="E5">
+        <v>48</v>
+      </c>
+      <c r="F5">
+        <v>47</v>
+      </c>
+      <c r="G5">
+        <v>4837</v>
+      </c>
+      <c r="H5">
+        <v>4741</v>
+      </c>
+      <c r="I5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J5">
+        <v>98.015000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>10</v>
       </c>
-      <c r="B3">
-        <v>2221</v>
-      </c>
-      <c r="C3">
-        <v>1170</v>
-      </c>
-      <c r="D3">
-        <v>1617</v>
-      </c>
-      <c r="E3">
-        <v>51</v>
-      </c>
-      <c r="F3">
-        <v>49</v>
-      </c>
-      <c r="G3">
-        <v>5172</v>
-      </c>
-      <c r="H3">
-        <v>4981</v>
-      </c>
-      <c r="I3">
-        <v>96.307000000000002</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B6">
+        <v>778</v>
+      </c>
+      <c r="C6">
+        <v>214</v>
+      </c>
+      <c r="D6">
+        <v>504</v>
+      </c>
+      <c r="E6">
+        <v>17</v>
+      </c>
+      <c r="F6">
+        <v>17</v>
+      </c>
+      <c r="G6">
+        <v>1701</v>
+      </c>
+      <c r="H6">
+        <v>1688</v>
+      </c>
+      <c r="I6" t="s">
+        <v>24</v>
+      </c>
+      <c r="J6">
+        <v>99.236000000000004</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>11</v>
       </c>
-      <c r="B4">
-        <v>852</v>
-      </c>
-      <c r="C4">
-        <v>221</v>
-      </c>
-      <c r="D4">
-        <v>494</v>
-      </c>
-      <c r="E4">
-        <v>17</v>
-      </c>
-      <c r="F4">
-        <v>17</v>
-      </c>
-      <c r="G4">
-        <v>1719</v>
-      </c>
-      <c r="H4">
-        <v>1692</v>
-      </c>
-      <c r="I4">
-        <v>98.429000000000002</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B7">
+        <v>857</v>
+      </c>
+      <c r="C7">
+        <v>177</v>
+      </c>
+      <c r="D7">
+        <v>495</v>
+      </c>
+      <c r="E7">
+        <v>15</v>
+      </c>
+      <c r="F7">
+        <v>15</v>
+      </c>
+      <c r="G7">
+        <v>1534</v>
+      </c>
+      <c r="H7">
+        <v>1527</v>
+      </c>
+      <c r="I7" t="s">
+        <v>25</v>
+      </c>
+      <c r="J7">
+        <v>99.543999999999997</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>12</v>
       </c>
-      <c r="B5">
-        <v>855</v>
-      </c>
-      <c r="C5">
-        <v>193</v>
-      </c>
-      <c r="D5">
-        <v>463</v>
-      </c>
-      <c r="E5">
+      <c r="B8">
+        <v>2015</v>
+      </c>
+      <c r="C8">
+        <v>1095</v>
+      </c>
+      <c r="D8">
+        <v>1566</v>
+      </c>
+      <c r="E8">
+        <v>53</v>
+      </c>
+      <c r="F8">
+        <v>53</v>
+      </c>
+      <c r="G8">
+        <v>5293</v>
+      </c>
+      <c r="H8">
+        <v>5290</v>
+      </c>
+      <c r="I8" t="s">
+        <v>20</v>
+      </c>
+      <c r="J8">
+        <v>99.942999999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9">
+        <v>867</v>
+      </c>
+      <c r="C9">
+        <v>198</v>
+      </c>
+      <c r="D9">
+        <v>511</v>
+      </c>
+      <c r="E9">
+        <v>13</v>
+      </c>
+      <c r="F9">
+        <v>12</v>
+      </c>
+      <c r="G9">
+        <v>1317</v>
+      </c>
+      <c r="H9">
+        <v>1249</v>
+      </c>
+      <c r="I9" t="s">
+        <v>23</v>
+      </c>
+      <c r="J9">
+        <v>94.837000000000003</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>14</v>
       </c>
-      <c r="F5">
-        <v>14</v>
-      </c>
-      <c r="G5">
-        <v>1458</v>
-      </c>
-      <c r="H5">
-        <v>1449</v>
-      </c>
-      <c r="I5">
-        <v>99.382999999999996</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6">
-        <v>1994</v>
-      </c>
-      <c r="C6">
-        <v>1135</v>
-      </c>
-      <c r="D6">
-        <v>1578</v>
-      </c>
-      <c r="E6">
-        <v>53</v>
-      </c>
-      <c r="F6">
-        <v>53</v>
-      </c>
-      <c r="G6">
-        <v>5454</v>
-      </c>
-      <c r="H6">
-        <v>5453</v>
-      </c>
-      <c r="I6">
-        <v>99.981999999999999</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7">
-        <v>859</v>
-      </c>
-      <c r="C7">
-        <v>247</v>
-      </c>
-      <c r="D7">
-        <v>525</v>
-      </c>
-      <c r="E7">
-        <v>13</v>
-      </c>
-      <c r="F7">
-        <v>13</v>
-      </c>
-      <c r="G7">
-        <v>1373</v>
-      </c>
-      <c r="H7">
-        <v>1297</v>
-      </c>
-      <c r="I7">
-        <v>94.465000000000003</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="B10">
+        <v>661</v>
+      </c>
+      <c r="C10">
+        <v>93</v>
+      </c>
+      <c r="D10">
+        <v>360</v>
+      </c>
+      <c r="E10">
+        <v>9</v>
+      </c>
+      <c r="F10">
+        <v>7</v>
+      </c>
+      <c r="G10">
+        <v>860</v>
+      </c>
+      <c r="H10">
+        <v>717</v>
+      </c>
+      <c r="I10" t="s">
+        <v>26</v>
+      </c>
+      <c r="J10">
+        <v>83.372</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>15</v>
       </c>
-      <c r="B8">
-        <v>640</v>
-      </c>
-      <c r="C8">
-        <v>86</v>
-      </c>
-      <c r="D8">
-        <v>364</v>
-      </c>
-      <c r="E8">
-        <v>9</v>
-      </c>
-      <c r="F8">
-        <v>7</v>
-      </c>
-      <c r="G8">
-        <v>893</v>
-      </c>
-      <c r="H8">
-        <v>739</v>
-      </c>
-      <c r="I8">
-        <v>82.754999999999995</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9">
-        <v>1358</v>
-      </c>
-      <c r="C9">
-        <v>505</v>
-      </c>
-      <c r="D9">
-        <v>896</v>
-      </c>
-      <c r="E9">
+      <c r="B11">
+        <v>1363</v>
+      </c>
+      <c r="C11">
+        <v>564</v>
+      </c>
+      <c r="D11">
+        <v>903</v>
+      </c>
+      <c r="E11">
         <v>24</v>
       </c>
-      <c r="F9">
+      <c r="F11">
         <v>22</v>
       </c>
-      <c r="G9">
-        <v>2413</v>
-      </c>
-      <c r="H9">
-        <v>2291</v>
-      </c>
-      <c r="I9">
-        <v>94.943999999999988</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10">
-        <v>1848</v>
-      </c>
-      <c r="C10">
-        <v>896</v>
-      </c>
-      <c r="D10">
-        <v>1307</v>
-      </c>
-      <c r="E10">
-        <v>41</v>
-      </c>
-      <c r="F10">
-        <v>40</v>
-      </c>
-      <c r="G10">
-        <v>4141</v>
-      </c>
-      <c r="H10">
-        <v>4037</v>
-      </c>
-      <c r="I10">
-        <v>97.489000000000004</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11">
-        <v>304</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <v>91</v>
-      </c>
-      <c r="E11">
-        <v>3</v>
-      </c>
-      <c r="F11">
-        <v>2</v>
-      </c>
       <c r="G11">
-        <v>269</v>
+        <v>2368</v>
       </c>
       <c r="H11">
-        <v>242</v>
-      </c>
-      <c r="I11">
-        <v>89.963000000000008</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12">
-        <v>44</v>
-      </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
-      <c r="G12">
-        <v>1</v>
-      </c>
-      <c r="H12">
-        <v>1</v>
-      </c>
-      <c r="I12">
-        <v>100</v>
+        <v>2250</v>
+      </c>
+      <c r="I11" t="s">
+        <v>22</v>
+      </c>
+      <c r="J11">
+        <v>95.016999999999996</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:J25" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J25">
+      <sortCondition ref="A1:A25"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>